<commit_message>
Renaming data files, adding to analysis of data
</commit_message>
<xml_diff>
--- a/src/Analysis/ExperimentalData/Results.xlsx
+++ b/src/Analysis/ExperimentalData/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\ULTRA\ThrustStudies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\ULTRA\batoid-burt-3\src\Analysis\ExperimentalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Voltage Amplitude</t>
   </si>
@@ -29,22 +29,7 @@
     <t>Mass (g)</t>
   </si>
   <si>
-    <t>Experiment 1</t>
-  </si>
-  <si>
-    <t>frequency (rad/s)</t>
-  </si>
-  <si>
     <t>Force (N)</t>
-  </si>
-  <si>
-    <t>f (Hz)</t>
-  </si>
-  <si>
-    <t>Experiment 2</t>
-  </si>
-  <si>
-    <t>Max Wave Amplitude (degrees)</t>
   </si>
   <si>
     <t>V_avg_steady</t>
@@ -239,11 +224,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="277424720"/>
-        <c:axId val="277425280"/>
+        <c:axId val="190523600"/>
+        <c:axId val="190524160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="277424720"/>
+        <c:axId val="190523600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -272,12 +257,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277425280"/>
+        <c:crossAx val="190524160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277425280"/>
+        <c:axId val="190524160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,7 +293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277424720"/>
+        <c:crossAx val="190523600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -325,7 +310,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -342,29 +327,209 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Amplitude vs. Avg of Min Forces</a:t>
+              <a:t>Sensor Calibration</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Force (N)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.19620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39141899999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58663799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78185700000000014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="193946080"/>
+        <c:axId val="193946640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="193946080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193946640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="193946640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193946080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -426,44 +591,117 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$7:$B$10</c:f>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.19620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>0.39141899999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>0.58663799999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>0.78185700000000014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$H$7:$H$10</c:f>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-0.20560954100000001</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.45893902400000003</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.46040902100000003</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.64170865099999996</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,11 +716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="749359424"/>
-        <c:axId val="749358864"/>
+        <c:axId val="675800144"/>
+        <c:axId val="675799584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="749359424"/>
+        <c:axId val="675800144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,12 +777,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749358864"/>
+        <c:crossAx val="675799584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="749358864"/>
+        <c:axId val="675799584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749359424"/>
+        <c:crossAx val="675800144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -650,640 +888,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sensor Calibration</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Force (N)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4.4999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.19620000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.39141899999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.58663799999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.78185700000000014</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="277427520"/>
-        <c:axId val="277428080"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="277427520"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Voltage Amplitude</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277428080"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="277428080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Force (N)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277427520"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400"/>
-              <a:t>Effect of Frequency</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" baseline="0"/>
-              <a:t> on Max Postive Force</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1400"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>f (Hz)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$20:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.63661977236758138</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95492965855137202</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2732395447351628</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5915494309189535</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.909859317102744</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$20:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.50929900000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1952976</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6942925</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.6742904999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2442975000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="277430320"/>
-        <c:axId val="277430880"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="277430320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Frequency (Hz)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277430880"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="277430880"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Force </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>(N)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277430320"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400"/>
-              <a:t>Effect of</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" baseline="0"/>
-              <a:t> Amplitude on Max Positive Force</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1400"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Force (N)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$34:$A$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$34:$B$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.99929800000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.2242954999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.2042934999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.4492929999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="37940480"/>
-        <c:axId val="37933760"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="37940480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Max Amplitude</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (Degrees)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37933760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="37933760"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Force</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>(N)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37940480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1447,11 +1052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274624032"/>
-        <c:axId val="274623472"/>
+        <c:axId val="193954480"/>
+        <c:axId val="193955040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274624032"/>
+        <c:axId val="193954480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,12 +1113,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274623472"/>
+        <c:crossAx val="193955040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="274623472"/>
+        <c:axId val="193955040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274624032"/>
+        <c:crossAx val="193954480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1619,7 +1224,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1777,11 +1382,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="753709088"/>
-        <c:axId val="753708528"/>
+        <c:axId val="193957280"/>
+        <c:axId val="193957840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="753709088"/>
+        <c:axId val="193957280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1838,12 +1443,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753708528"/>
+        <c:crossAx val="193957840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="753708528"/>
+        <c:axId val="193957840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,7 +1505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753709088"/>
+        <c:crossAx val="193957280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1949,7 +1554,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2113,11 +1718,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="746663696"/>
-        <c:axId val="749500000"/>
+        <c:axId val="193960080"/>
+        <c:axId val="193960640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="746663696"/>
+        <c:axId val="193960080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2174,12 +1779,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749500000"/>
+        <c:crossAx val="193960640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="749500000"/>
+        <c:axId val="193960640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,7 +1841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="746663696"/>
+        <c:crossAx val="193960080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2285,7 +1890,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2443,11 +2048,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="755076432"/>
-        <c:axId val="749498880"/>
+        <c:axId val="662725344"/>
+        <c:axId val="662725904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="755076432"/>
+        <c:axId val="662725344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2504,12 +2109,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749498880"/>
+        <c:crossAx val="662725904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="749498880"/>
+        <c:axId val="662725904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2566,7 +2171,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="755076432"/>
+        <c:crossAx val="662725344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2615,7 +2220,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2779,11 +2384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="760321472"/>
-        <c:axId val="760320912"/>
+        <c:axId val="662728144"/>
+        <c:axId val="662728704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="760321472"/>
+        <c:axId val="662728144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2840,12 +2445,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="760320912"/>
+        <c:crossAx val="662728704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="760320912"/>
+        <c:axId val="662728704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2902,7 +2507,332 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="760321472"/>
+        <c:crossAx val="662728144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Amplitude vs. Avg of Min Forces</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$7:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$7:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-0.20560954100000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.45893902400000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.46040902100000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.64170865099999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="662730944"/>
+        <c:axId val="662731504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="662730944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="662731504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="662731504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="662730944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3191,6 +3121,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5772,6 +5742,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6351,20 +6837,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6379,36 +6865,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6417,15 +6873,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6884,10 +7340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A37"/>
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6900,7 +7356,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6949,169 +7405,6 @@
       <c r="C5">
         <f>A5*9.81/1000</f>
         <v>0.78185700000000014</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>0.1</v>
-      </c>
-      <c r="C20">
-        <f>4.89999*B20+0.0193</f>
-        <v>0.50929900000000006</v>
-      </c>
-      <c r="D20">
-        <f>A20/(2*PI())</f>
-        <v>0.63661977236758138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>0.24</v>
-      </c>
-      <c r="C21">
-        <f>4.89999*B21+0.0193</f>
-        <v>1.1952976</v>
-      </c>
-      <c r="D21">
-        <f>A21/(2*PI())</f>
-        <v>0.95492965855137202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8</v>
-      </c>
-      <c r="B22">
-        <v>0.75</v>
-      </c>
-      <c r="C22">
-        <f>4.89999*B22+0.0193</f>
-        <v>3.6942925</v>
-      </c>
-      <c r="D22">
-        <f>A22/(2*PI())</f>
-        <v>1.2732395447351628</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23">
-        <v>0.95</v>
-      </c>
-      <c r="C23">
-        <f>4.89999*B23+0.0193</f>
-        <v>4.6742904999999997</v>
-      </c>
-      <c r="D23">
-        <f>A23/(2*PI())</f>
-        <v>1.5915494309189535</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>12</v>
-      </c>
-      <c r="B24">
-        <v>0.25</v>
-      </c>
-      <c r="C24">
-        <f>4.89999*B24+0.0193</f>
-        <v>1.2442975000000001</v>
-      </c>
-      <c r="D24">
-        <f>A24/(2*PI())</f>
-        <v>1.909859317102744</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34">
-        <f>4.89999*C34+0.0193</f>
-        <v>0.99929800000000002</v>
-      </c>
-      <c r="C34">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>6</v>
-      </c>
-      <c r="B35">
-        <f>4.89999*C35+0.0193</f>
-        <v>2.2242954999999998</v>
-      </c>
-      <c r="C35">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>9</v>
-      </c>
-      <c r="B36">
-        <f>4.89999*C36+0.0193</f>
-        <v>3.2042934999999999</v>
-      </c>
-      <c r="C36">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>12</v>
-      </c>
-      <c r="B37">
-        <f>4.89999*C37+0.0193</f>
-        <v>3.4492929999999995</v>
-      </c>
-      <c r="C37">
-        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -7125,7 +7418,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7137,28 +7430,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -7172,7 +7465,7 @@
         <v>-3.8999999999999998E-3</v>
       </c>
       <c r="D2">
-        <f>4.89999*C2+0.0193</f>
+        <f t="shared" ref="D2:D10" si="0">4.89999*C2+0.0193</f>
         <v>1.9003900000000296E-4</v>
       </c>
       <c r="E2">
@@ -7201,21 +7494,21 @@
         <v>5.1799999999999999E-2</v>
       </c>
       <c r="D3">
-        <f>4.89999*C3+0.0193</f>
+        <f t="shared" si="0"/>
         <v>0.27311948199999997</v>
       </c>
       <c r="E3">
         <v>0.1116</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F10" si="0">4.89999*E3+0.0193</f>
+        <f t="shared" ref="F3:F10" si="1">4.89999*E3+0.0193</f>
         <v>0.56613888400000001</v>
       </c>
       <c r="G3">
         <v>-5.2600000000000001E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="1">4.89999*G3+0.0193</f>
+        <f t="shared" ref="H3:H10" si="2">4.89999*G3+0.0193</f>
         <v>-0.23843947400000001</v>
       </c>
     </row>
@@ -7230,21 +7523,21 @@
         <v>0.08</v>
       </c>
       <c r="D4">
-        <f>4.89999*C4+0.0193</f>
+        <f t="shared" si="0"/>
         <v>0.41129919999999998</v>
       </c>
       <c r="E4">
         <v>0.31740000000000002</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.574556826</v>
       </c>
       <c r="G4">
         <v>-8.8300000000000003E-2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.41336911700000001</v>
       </c>
     </row>
@@ -7259,21 +7552,21 @@
         <v>6.83E-2</v>
       </c>
       <c r="D5">
-        <f>4.89999*C5+0.0193</f>
+        <f t="shared" si="0"/>
         <v>0.35396931699999995</v>
       </c>
       <c r="E5">
         <v>0.31850000000000001</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.579946815</v>
       </c>
       <c r="G5">
         <v>-0.21410000000000001</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.029787859</v>
       </c>
     </row>
@@ -7288,27 +7581,27 @@
         <v>4.2799999999999998E-2</v>
       </c>
       <c r="D6">
-        <f>4.89999*C6+0.0193</f>
+        <f t="shared" si="0"/>
         <v>0.229019572</v>
       </c>
       <c r="E6">
         <v>0.14960000000000001</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75233850400000002</v>
       </c>
       <c r="G6">
         <v>-9.4500000000000001E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.443749055</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -7317,27 +7610,27 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="D7">
-        <f>4.89999*C7+0.0193</f>
+        <f t="shared" si="0"/>
         <v>7.1729893000000003E-2</v>
       </c>
       <c r="E7">
         <v>8.77E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.44902912299999997</v>
       </c>
       <c r="G7">
         <v>-4.5900000000000003E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.20560954100000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -7346,27 +7639,27 @@
         <v>1.43E-2</v>
       </c>
       <c r="D8">
-        <f>4.89999*C8+0.0193</f>
+        <f t="shared" si="0"/>
         <v>8.9369856999999997E-2</v>
       </c>
       <c r="E8">
         <v>0.25080000000000002</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2482174920000002</v>
       </c>
       <c r="G8">
         <v>-9.7600000000000006E-2</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.45893902400000003</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -7375,27 +7668,27 @@
         <v>5.0099999999999999E-2</v>
       </c>
       <c r="D9">
-        <f>4.89999*C9+0.0193</f>
+        <f t="shared" si="0"/>
         <v>0.26478949899999998</v>
       </c>
       <c r="E9">
         <v>0.30780000000000002</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5275169220000002</v>
       </c>
       <c r="G9">
         <v>-9.7900000000000001E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.46040902100000003</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -7404,21 +7697,21 @@
         <v>6.1499999999999999E-2</v>
       </c>
       <c r="D10">
-        <f>4.89999*C10+0.0193</f>
+        <f t="shared" si="0"/>
         <v>0.32064938499999995</v>
       </c>
       <c r="E10">
         <v>0.2802</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3922771980000002</v>
       </c>
       <c r="G10">
         <v>-0.13489999999999999</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.64170865099999996</v>
       </c>
     </row>

</xml_diff>